<commit_message>
Cost mise en place fasteners,...
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/SU/SUA0100_to_SUA0400.xlsx
+++ b/CR - Cost Report/BOM/SU/SUA0100_to_SUA0400.xlsx
@@ -620,7 +620,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>31</v>
@@ -781,7 +781,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>32</v>

</xml_diff>